<commit_message>
load_news now generates news.json and main loads from it.
</commit_message>
<xml_diff>
--- a/news.xlsx
+++ b/news.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -662,7 +662,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>17 hours ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -730,42 +730,42 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.theglobeandmail.com/investing/markets/markets-news/GetNews/27431899/neareye-display-market-size-projected-to-reach-usd-53-billion-by-2027-at-a-cagr-of-247</t>
+          <t>https://www.digitimes.com/news/a20240710PD218/microled-apple-automotive-lidar-demand.html</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The Globe and Mail</t>
+          <t>Ams Osram sees promising automotive microLED and LiDAR demand outlook</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>The global Near-Eye Display (NED) Market is anticipated to achieve 
-remarkable growth, with its market size projected to reach USD 5.3 billion 
-by 2027,...</t>
+          <t>Apple sent shock waves across the industry in March by canceling its 
+microLED project and ending collaboration with Ams OSRAM.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>11 hours ago</t>
+          <t>6 days ago</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>The Globe and Mail</t>
+          <t>digitimes</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.ryt9.com/en/prg/277286</t>
+          <t>https://www.newswit.com/en/ifb2vntjeewr5ezf74wqsbqzv2ov3t19</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
           <t>LG partners with mo-sys, empowering thai talents in production industry and 
-corporate customers to</t>
+corporate customers to create world-class content with cutting-edge tech at 
+mo-sys academy bangkok</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -782,119 +782,91 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>RYT9</t>
+          <t>newswit</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.digitimes.com/news/a20240710PD218/microled-apple-automotive-lidar-demand.html</t>
+          <t>https://www.northernnews.ca/newsfile/216626-vuereal-scales-microsolid-printing-doubles-production-facility-strengthens-leadership-for-automotive-and-consumer-innovation-2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ams Osram sees promising automotive microLED and LiDAR demand outlook</t>
+          <t>VueReal Scales MicroSolid Printing: Doubles Production Facility</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
-        <is>
-          <t>Apple sent shock waves across the industry in March by canceling its 
-microLED project and ending collaboration with Ams OSRAM.</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>6 days ago</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>digitimes</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>https://www.northernnews.ca/newsfile/216626-vuereal-scales-microsolid-printing-doubles-production-facility-strengthens-leadership-for-automotive-and-consumer-innovation-2</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>VueReal Scales MicroSolid Printing: Doubles Production Facility</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
         <is>
           <t>Waterloo, Ontario–(Newsfile Corp. – July 16, 2024) – VueReal, a pioneer in 
 MicroSolid Printing technology, today unveiled plans for a significant 
 expansion...</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>21 hours ago</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Northern News</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://www.digitimes.com/news/a20240710PD213.html?chid=10</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Chinese AI models show strength and resilience amid US sanctions</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Chinese AI companies showcased resilience and innovation at the 2024 World 
+AI Conference (WAIC 2024) amid the US's tightening AI chip export sanctions.</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>19 hours ago</t>
+          <t>6 days ago</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Northern News</t>
+          <t>digitimes</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.digitimes.com/news/a20240710PD213.html?chid=10</t>
+          <t>https://www.retail4growth.com/news/immersive-led-feel-at-unilumins-new-experience-centre-6820</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Chinese AI models show strength and resilience amid US sanctions</t>
+          <t>Immersive LED feel at Unilumin's new experience centre</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
-        <is>
-          <t>Chinese AI companies showcased resilience and innovation at the 2024 World 
-AI Conference (WAIC 2024) amid the US's tightening AI chip export sanctions.</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>6 days ago</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>digitimes</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>https://www.retail4growth.com/news/immersive-led-feel-at-unilumins-new-experience-centre-6820</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Immersive LED feel at Unilumin's new experience centre</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
         <is>
           <t>Unilumin has just opened its first state-of-the-art experience centre in 
 Noida, which showcases the latest LED COB and MIP technologies and products 
 with an...</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>6 days ago</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>Retail4growth</t>
         </is>
@@ -967,7 +939,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1 day ago</t>
+          <t>2 days ago</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1083,7 +1055,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>20 hours ago</t>
+          <t>22 hours ago</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1269,58 +1241,58 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>https://www.techtimes.com/articles/306659/20240714/wearable-tech-helps-scientists-track-study-the-impact-of-stress-during-sleep.htm</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Wearable Tech Helps Scientists Track &amp; Study the Impact of Stress During 
+Sleep</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Wearable technology—from smartwatches to virtual reality devices the last 
+ten years has seen an explosion in innovation across the sector.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2 days ago</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Tech Times</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>https://www.businessinsider.com/guides/tech/how-to-preorder-the-samsung-galaxy-ring-2024-7</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>How to Preorder the Samsung Galaxy Ring, a New Wearable Health-Tracker</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>Samsung's new Galaxy Ring is finally available for preorder. Designed as a 
 competitor to the Oura Ring, the new device is a health-tracking wearable 
 that...</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>6 days ago</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>Business Insider</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>https://www.techtimes.com/articles/306659/20240714/wearable-tech-helps-scientists-track-study-the-impact-of-stress-during-sleep.htm</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Wearable Tech Helps Scientists Track &amp; Study the Impact of Stress During 
-Sleep</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Wearable technology—from smartwatches to virtual reality devices the last 
-ten years has seen an explosion in innovation across the sector.</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>2 days ago</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Tech Times</t>
         </is>
       </c>
     </row>
@@ -1373,7 +1345,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>4 days ago</t>
+          <t>5 days ago</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1385,436 +1357,437 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.citizentribune.com/news/business/samsung-brings-techs-latest-fashion-to-wearable-technology-with-ai-twists-in-new-watch-and/article_e9e63447-eb75-57f9-8ce8-032c532e5d45.html</t>
+          <t>https://www.hospimedica.com/critical-care/articles/294801839/ai-integrated-wearable-sensor-accurately-measures-step-length-for-evaluation-of-neurological-diseases.html</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Samsung brings tech's latest fashion to wearable technology with AI twists 
-in new watch and ring</t>
+          <t>AI-Integrated Wearable Sensor Accurately Measures Step Length for 
+Evaluation of Neurological Diseases</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Samsung is dressing up its wearable devices in technology's latest fashion 
-— artificial intelligence. The South Korean electronics giant on 
-Wednesday...</t>
+          <t>Step length is recognized as a sensitive and non-invasive metric for 
+assessing a variety of conditions and diseases such as aging,...</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6 days ago</t>
+          <t>20 hours ago</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Citizen Tribune</t>
+          <t>HospiMedica International</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.sportsbusinessjournal.com/Articles/2024/07/16/gorout-liberty-league</t>
+          <t>https://nocamels.com/2024/07/colorado-medicaid-provider-to-cover-israeli-wearable-for-migraines/</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>NCAA approves Liberty League to use in-game play calling technology from 
-GoRout</t>
+          <t>Colorado Medicaid Provider To Cover Israeli Wearable For Migraines</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>The Liberty League's seven teams institute GoRout's game system across 
-in-conference football games (and out-of-conference matchups if their 
-opponent...</t>
+          <t>Health First Colorado, the state's Medicaid provider, will provide coverage 
+for an Israeli-made wearable device for migraine relief.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>10 hours ago</t>
+          <t>6 days ago</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Sports Business Journal</t>
+          <t>NoCamels</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.hospimedica.com/critical-care/articles/294801839/ai-integrated-wearable-sensor-accurately-measures-step-length-for-evaluation-of-neurological-diseases.html</t>
+          <t>https://medicalxpress.com/news/2024-07-shelf-wearable-trackers-clinically-patients.html</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>AI-Integrated Wearable Sensor Accurately Measures Step Length for 
-Evaluation of Neurological Diseases</t>
+          <t>Off-the-shelf wearable trackers provide clinically-useful information for 
+patients with heart disease</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Step length is recognized as a sensitive and non-invasive metric for 
-assessing a variety of conditions and diseases such as aging,...</t>
+          <t>A study published in Nature Medicine examined if a commercially-available 
+fitness tracker and smartphone could continuously monitor the response to...</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18 hours ago</t>
+          <t>1 day ago</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>HospiMedica International</t>
+          <t>Medical Xpress</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://nocamels.com/2024/07/colorado-medicaid-provider-to-cover-israeli-wearable-for-migraines/</t>
+          <t>https://www.forbes.com/sites/forbes-personal-shopper/article/best-fitness-trackers/</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Colorado Medicaid Provider To Cover Israeli Wearable For Migraines</t>
+          <t>The 7 Best Fitness Trackers, Tested By A Personal Trainer</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
-        <is>
-          <t>Health First Colorado, the state's Medicaid provider, will provide coverage 
-for an Israeli-made wearable device for migraine relief.</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>6 days ago</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>NoCamels</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>https://marketscale.com/industries/education-technology/why-hardwired-buttons-outperform-wearable-devices-in-school-safety/</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Why Hardwired Buttons Outperform Wearable Devices in School Safety</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>A recent "Secured" episode highlighted the need to upgrade school safety 
-systems from outdated analog intercoms to IP-based solutions.</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>1 day ago</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>MarketScale</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>https://medicalxpress.com/news/2024-07-shelf-wearable-trackers-clinically-patients.html</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Off-the-shelf wearable trackers provide clinically-useful information for 
-patients with heart disease</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>A study published in Nature Medicine examined if a commercially-available 
-fitness tracker and smartphone could continuously monitor the response to...</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>1 day ago</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Medical Xpress</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>https://www.forbes.com/sites/forbes-personal-shopper/article/best-fitness-trackers/</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>The 7 Best Fitness Trackers, Tested By A Personal Trainer</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
         <is>
           <t>The best fitness trackers can guide you to reach your health goals. I've 
 spent four months testing 14 different wearables to find the best fitness 
 trackers...</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>5 days ago</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>Forbes</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="21">
+      <c r="A21" t="inlineStr">
         <is>
           <t>https://www.globenewswire.com/news-release/2024/07/11/2911971/32656/en/Wearable-AI-Market-is-expected-to-Grow-at-an-8-3-CAGR-and-Reach-USD-146-2-billion-by-2034-Report-by-Transparency-Market-Research-Inc.html</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>Wearable AI Market is expected to Grow at an 8.3% CAGR and</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>AI-powered wearables offer customized fitness plans and real-time coaching, 
 adapting to individual goals and progress....</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>5 days ago</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>GlobeNewswire</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://www.digitimes.com/news/a20240717PD218/samsung-wearable-demand-sales-galaxy.html</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>With wearable device demand declining, Samsung lays out plans to boost sales</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Despite a decline in demand for devices like smartwatches in the first half 
+of the year, Samsung remains hopeful that new products and marketing 
+strategies...</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>3 hours ago</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>digitimes</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
         <is>
           <t>https://www.globenewswire.com/news-release/2024/07/15/2913085/0/en/Wearable-Devices-Unveils-Innovative-ChatGPT-Gestures-Interaction-for-Apple-Watch-Using-Mudra-Band-Enhancing-AI-Integration.html</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>Wearable Devices Unveils Innovative ChatGPT Gestures</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>The new user experience enables interaction with AI agents through 
 touchless gestures, offering a seamless and innovative way to engage with 
 AI technology -.</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>1 day ago</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>GlobeNewswire</t>
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>https://www.digitimes.com/news/a20240717PD218/samsung-wearable-demand-sales-galaxy.html</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>With wearable device demand declining, Samsung lays out plans to boost sales</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Despite a decline in demand for devices like smartwatches in the first half 
-of the year, Samsung remains hopeful that new products and marketing 
-strategies...</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>54 minutes ago</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>digitimes</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="24">
+      <c r="A24" t="inlineStr">
         <is>
           <t>https://www.stocktitan.net/news/WLDS/wearable-devices-unveils-the-revolutionary-mudra-link-the-first-ai-2nqborjfhrn0.html</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>Wearable Devices Unveils the Revolutionary Mudra LINK: The First AI Neural 
 Interface Wristband for Android and Beyond</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>Wearable Devices (Nasdaq: WLDS) has unveiled the Mudra LINK, an AI-powered 
 neural wristband for Bluetooth-enabled devices.</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>20 hours ago</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>22 hours ago</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>Stock Titan</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+    <row r="25">
+      <c r="A25" t="inlineStr">
         <is>
           <t>https://news.samsung.com/global/samsungs-expanded-wearables-portfolio-unlocks-intelligent-health-experiences-for-all</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>Samsung’s Expanded Wearables Portfolio Unlocks Intelligent Health 
 Experiences for All</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>Samsung Galaxy Ring, Galaxy Watch7 and Galaxy Watch Ultra enable new, 
 intelligent health experiences across the portfolio, making everyday 
 wellness more...</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>6 days ago</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>Samsung Global Newsroom</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
+    <row r="26">
+      <c r="A26" t="inlineStr">
         <is>
           <t>https://www.zdnet.com/article/best-fitness-ring/</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>The best fitness rings of 2024: Expert tested and reviewed</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>We tested the top smart rings on the market from Oura, Ultrahuman, and 
 more, to help you choose the best ring for you, no matter how you exercise.</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>6 days ago</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>ZDNET</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>ZDNet</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
         <is>
           <t>https://finance.yahoo.com/news/sports-analytics-market-size-worth-173900140.html</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>Sports Analytics Market Size Worth US$ 20.48 Billion By 2032 With a CAGR of 
 22.51%, Boosted by Surged Usage of Wearable Technology | Research by SNS 
 Insider</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>The Sports Analytics Market is Experiencing Robust Growth by Raising 
 Emphasis on Real-Time Data for Organizing Training Sessions, Says SNS 
 Insider,...</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>4 days ago</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Yahoo Finance</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://abcnews.go.com/GMA/Wellness/samsung-unveils-1st-smart-ring-biometric-health-monitoring/story?id=111849999</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Samsung unveils 1st smart ring with biometric health monitoring, how it 
+stacks up to the Oura Ring</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>What to know about the new Samsung Galaxy Ring, Samsung's new wearable 
+technology device with 24/7 health monitoring capabilities.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>5 days ago</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>ABC News - Breaking News, Latest News and Videos</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://www.msn.com/en-xl/news/other/wearable-technology-the-wearable-smart-devices-that-are-changing-our-daily-lives/ss-BB1pTff8?ocid=finance-verthp-feeds</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Wearable technology: the wearable smart devices that are changing our daily 
+lives</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>The link between fashion and the technology sector has a long history, 
+culminating in wearable technology products that have changed or will 
+significantly...</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>3 days ago</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>MSN</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>https://www.msn.com/en-us/news/technology/self-assembling-highly-conductive-sensors-could-improve-wearable-devices/ar-BB1oZSyV?item=flightsprg-tipsubsc-v1a?season=2024/</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Self-assembling, highly conductive sensors could improve wearable devices</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Penn State researchers developed a new soft and stretchable material that 
+can be 3D-printed. The material can be used to fabricate wearable 
+devices,...</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4 days ago</t>
+          <t>22 hours ago</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Yahoo Finance</t>
+          <t>MSN</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://finance.yahoo.com/news/samsungs-galaxy-ring-smart-device-093000311.html</t>
+          <t>https://www.insideprecisionmedicine.com/topics/translational-research/popular-wearables-can-help-doctors-manage-medication-in-patients-with-heart-disease/</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Can Samsung's new Galaxy Ring smart device help its China comeback?</t>
+          <t>Popular Wearables Can Help Doctors Manage Medication in Patients with Heart 
+Disease</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Samsung Electronics, once the dominant smartphone player in China, is 
-drawing fresh interest from consumers on the mainland after the South 
-Korean tech...</t>
+          <t>A new study suggests doctors can use information from their patients' 
+wearable devices to monitor the effectiveness of medications they prescribe 
+to treat...</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>5 days ago</t>
+          <t>1 day ago</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Yahoo Finance</t>
+          <t>Inside Precision Medicine</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2030,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>18 hours ago</t>
+          <t>20 hours ago</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -2174,867 +2147,868 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>https://www.engadget.com/best-vr-headsets-140012529.html</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>The best VR headsets for 2024</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>If you've been intrigued by virtual reality for a while, there are a number 
+of solid headsets to consider. These are the best VR headsets we've tested 
+and...</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>6 days ago</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Engadget</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>https://www.livescience.com/prime-day-vr-headset-deal-meta-quest-3-now-discounted</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Slip into VR for less with this Meta Quest 3 Prime Day deal</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Virtual Reality may not quite have hit the mainstream in the same way 
 traditional video games have, but if it does, it'll have a lot to thank the 
 Meta Quest...</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>16 hours ago</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>18 hours ago</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Live Science</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>https://www.digitimes.com/news/a20240710VL203/3d-ar_vr-display-lcd-technology.html</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Rain Technology to revolutionize AR/VR displays with brightness and FOV 
 breakthroughs</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>US-based Rain Technology has accumulated more than two decades of 
 experience in consumer display technologies, with ventures into LCD, OLED, 
 e-privacy,...</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>1 week ago</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>digitimes</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>https://omdia.tech.informa.com/pr/2024/jul/new-omdia-research-highlights-near-eye-display-market-poised-for-growth-as-leading-brands-revive-sales-efforts</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>New Omdia research highlights near-eye display market poised for growth as 
 leading brands revive sales efforts</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Stay informed on the XR market trends with new research from Omdia. Despite 
 a slowdown, top brands are focused on driving growth in AR, VR,...</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>6 days ago</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Omdia</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>https://www.macworld.com/article/557878/apple-vision-pro-features-specs-price-faq.html</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Apple Vision Pro guide: Everything you need to know</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Having launched in the U.S. in February, Apple Vision Pro is now available 
+to buy in the U.K., Canada and elsewhere. Here's what you should know 
+about...</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>4 days ago</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Macworld</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>https://www.geekwire.com/2024/new-virtual-reality-gaming-and-entertainment-venue-mirra-opening-in-bellevue/</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>New virtual reality gaming and entertainment venue Mirra opening in Bellevue</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>(Mirra Image) Virtual reality entertainment startup Mirra plans to open its 
 first location in Bellevue, Wash. in August. Mirra is a “social 
 entertainment.</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>17 hours ago</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>19 hours ago</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>GeekWire</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>https://www.roadtovr.com/somnium-vr1-hands-on/</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>Somnium VR1 Hands-on: Enthusiast Level PC VR at a Difficult Price Point</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Somnium VR1 is a new PC VR headset that delivers an impressive 
 field-of-view (FOV) and high-resolution displays, ideally appealing to 
 enthusiasts already in...</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>1 day ago</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Road to VR</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>https://www.ign.com/articles/best-vr-headset</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>Best VR Headset in 2024</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>We dive into the deep end of virtual reality to bring you the best VR 
 headsets, which we've all rigorously tested.</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>1 week ago</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>IGN</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>https://www.prnewswire.com/news-releases/arvrmr-market-revolutionizing-industries-pathway-to-surpassing-usd-521-28-billion-by-2031--skyquest-302198168.html</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>AR/VR/MR Market Revolutionizing Industries: Pathway to Surpassing USD 
 521.28 Billion by 2031 | SkyQuest</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>PRNewswire/ -- According to SkyQuest, the global, AR/VR/MR Market size was 
 valued at USD 30.6 Billion in 2022 and is poised to grow from USD 42.46 
 Billion...</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>18 hours ago</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>20 hours ago</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>PR Newswire</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://tvnewscheck.com/tech/article/local-tv-widens-embrace-of-virtual-sets-ar-vr/</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Local TV Stations Widen Their Embrace Of Virtual Sets, AR &amp; VR</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CBS-owned KPIX, Hearst's WCVB and a growing number of TelevisaUnivision 
+stations are among those leaning into virtual sets and expanding use of AR 
+and VR...</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>6 days ago</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>TV News Check</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
         <is>
           <t>https://www.trendhunter.com/trends/goovis-art</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>Ultra-Wide Head-Mounted Displays</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>GOOVIS ART - The GOOVIS ART ultra-wide head-mounted display is the brand's 
 latest wearable engineered with a next-generation experience in mind. The 
 heads.</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>3 days ago</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>Trend Hunter</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="13">
+      <c r="A13" t="inlineStr">
         <is>
           <t>https://www.analyticsinsight.net/gaming/top-vr-headsets-for-gaming-in-2024</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>Top VR Headsets for Gaming in 2024</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>As the gaming industry continues to explode, virtual reality gaming has 
 made a major advancement over the years. VR headsets offers engaging 
 gaming...</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>4 days ago</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5 days ago</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>Analytics Insight</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>https://www.zdnet.com/article/i-returned-my-apple-vision-pro-and-meta-quest-3-for-these-xr-glasses-and-theyre-30-off-for-prime-day/</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>I returned my Apple Vision Pro and Meta Quest 3 for these XR glasses - and 
 they're 30% off for Prime Day</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>The Viture One XR glasses expand your viewing experience and are now just 
 $299 for Amazon Prime Day.</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>21 hours ago</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>ZDNET</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>23 hours ago</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>ZDNet</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>https://www.telecomlead.com/smart-phone/xr-industry-developments-and-near-eye-display-market-outlook-117090</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>XR industry developments and near-eye display market outlook</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Kimi Lin and a team of analysts at Omdia have published a report on the 
 growth potential of the near-eye display market.</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>5 days ago</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>TelecomLead</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="16">
+      <c r="A16" t="inlineStr">
         <is>
           <t>https://uk.pcmag.com/laptops/95117/the-best-laptops-for-vr-in-2020</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>The Best Laptops for VR in 2024</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>Today's tethered virtual reality headsets demand a powerful PC. Don't want 
 to rely on a bulky desktop? These are the top notebooks we've tested that 
 have...</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>4 days ago</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>PCMag UK</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>https://ca.movies.yahoo.com/movies/2017-09-27-eve-valkyrie-warzone-no-vr-required.html</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>'Eve: Valkyrie' drops the VR requirement</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>If what's been holding you back from playing Eve: Valkyrie has been the 
 lack of a VR headset, that (very valid) reason has disappeared.</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>6 days ago</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>Yahoo Movies Canada</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="18">
+      <c r="A18" t="inlineStr">
         <is>
           <t>https://www.laptopmag.com/reviews/viture-pro-xr-smart-glasses</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>VITURE Pro XR Glasses review: These AR smart glasses add a new dimension to 
 Windows and Mac computers</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Smart glasses like the VITURE Pro XR give you instant access to a 135-inch 
 virtual display for laptops, phones, and tablets. But are they worth their 
 bold...</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>5 days ago</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>Laptop Mag</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="19">
+      <c r="A19" t="inlineStr">
         <is>
           <t>https://www.wicz.com/story/51022484/Laser-Display-Technology-Market-Is-Likely-to-Experience-a-Strong-Growth-During-2024-2032/</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>Laser Display Technology Market Is Likely to Experience a Strong Growth 
 During 2024-2032</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>Laser Display Technology Market Size 2024 To 2032 Laser Display Technology 
 Market Analysis [Latest 105 Report Pages with 20.12% CAGR]| by Product 
 Type...</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>6 days ago</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>WICZ</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://uk.pcmag.com/virtual-reality/75926/the-best-vr-headsets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>The Best VR Headsets for 2024</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Work or play in another dimension by donning one of the top-rated 
+standalone or tethered virtual reality headsets we've tested.</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>6 days ago</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>PCMag UK</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://au.pcmag.com/graphic-cards/52950/the-best-graphics-cards-for-vr-in-2020</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>The Best Graphics Cards for VR in 2024</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Building or upgrading a PC that you want to use with the latest virtual 
+reality headsets, but not sure which video card to buy? Here's what you 
+need to know...</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>4 days ago</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>PCMag Australia</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
         <is>
           <t>https://www.theglobeandmail.com/investing/markets/markets-news/GetNews/27431899/neareye-display-market-size-projected-to-reach-usd-53-billion-by-2027-at-a-cagr-of-247</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>The Globe and Mail</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>The global Near-Eye Display (NED) Market is anticipated to achieve 
 remarkable growth, with its market size projected to reach USD 5.3 billion 
 by 2027,...</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>11 hours ago</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>13 hours ago</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>The Globe and Mail</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>https://uk.pcmag.com/virtual-reality/75926/the-best-vr-headsets</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>The Best VR Headsets for 2024</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Work or play in another dimension by donning one of the top-rated 
-standalone or tethered virtual reality headsets we've tested.</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>6 days ago</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>PCMag UK</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>https://au.pcmag.com/graphic-cards/52950/the-best-graphics-cards-for-vr-in-2020</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>The Best Graphics Cards for VR in 2024</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Building or upgrading a PC that you want to use with the latest virtual 
-reality headsets, but not sure which video card to buy? Here's what you 
-need to know...</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>4 days ago</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>PCMag Australia</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+    <row r="23">
+      <c r="A23" t="inlineStr">
         <is>
           <t>https://www.livemint.com/technology/gadgets/best-wearables-to-buy-for-yourself-top-10-picks-for-you-to-adopt-a-wire-free-lifestyle-11720608242303.html</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>Best wearables to buy for yourself: Top 10 picks for you to adopt a 
 wire-free lifestyle | Mint</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>Check out the top wearables like smartwatches, headphones, neckband 
 earphones and more in our curated list. Choose from top brands and get the 
 one you have...</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>6 days ago</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>mint</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+    <row r="24">
+      <c r="A24" t="inlineStr">
         <is>
           <t>https://www.phonearena.com/ar-vr/reviews/xreal-air-2-pro-review_id6255</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>Xreal Air 2 Pro review: extra futuristic, thanks to this one (very useful) 
 gimmick</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>Are the Xreal Air 2 Pro worth the $449 (€515 in Europe), or should you 
 stick to the more affordable $399 Xreal Air instead? Let's find out…</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>1 day ago</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>PhoneArena</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>https://surgeradio.cl/ciencia-y-tecnologia/the-best-vr-headsets-for-2024/22045/</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>The best VR headsets for 2024</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>If you've been tempted to buy a VR headset after seeing the Apple Vision 
-Pro in action, you're not alone. And the best news is, you don't have to 
-spend...</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>5 days ago</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>surgeradio.cl</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://www.msn.com/en-us/news/technology/the-meta-quest-s-airplane-mode-is-nice-but-i-find-it-pointless/ar-BB1pPnwT?item=flightsprg-tipsubsc-v1aseason=2024/</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>The Meta Quest's airplane mode is nice, but I find it pointless</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Airplane mode recently launched on the Meta Quest, but the feature has one 
+big problem: VR headsets are just too big for travel.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>5 hours ago</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>MSN</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
         <is>
           <t>https://www.researchgate.net/publication/382224123_Deceptive_Modulation_of_Actual_and_Perceived_Effort_While_Walking_Using_Immersive_Virtual_Reality_A_Teleoanticipatory_Approach</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>Deceptive Modulation of Actual and Perceived Effort While</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>PDF | Virtual reality and technology-driven 'exergaming' have grown in 
 tandem to expand the possibilities of exercise. However, few studies have.</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>3 days ago</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>ResearchGate</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="27">
+      <c r="A27" t="inlineStr">
         <is>
           <t>https://www.msn.com/en-us/news/technology/full-amd-ryzen-pc-crammed-into-a-folding-mini-keyboard-includes-a-built-in-trackpad-and-battery-all-you-need-is-a-display/ar-BB1pyUEm?item=flights%3Cimg%20src&amp;item=flights%3Cimg%20src&amp;item=flights%3Cimg%20src&amp;item=flights%3Cimg%20src</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>Full AMD Ryzen PC crammed into a folding mini keyboard — includes a 
 built-in trackpad and battery; all you need is a display</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>Chinese PC maker Linglong has just introduced a tiny PC that fits into a 
 foldable keyboard. The company shared its live presentation, where the 
 presenter...</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>5 days ago</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>MSN</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>https://www.msn.com/en-us/lifestyle/shopping/this-giant-samsung-monitor-is-720-off-before-prime-day/ar-BB1q2Mfk?item=themed_featuredapps_enabled?loadin=defaultbrowser</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://www.msn.com/en-us/lifestyle/shopping/this-giant-samsung-monitor-is-720-off-before-prime-day/ar-BB1q2Mfk?item=flightsprg-tipsubsc-v1a?season=2024/</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>This giant Samsung monitor is $720 off before Prime Day</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>The Samsung Odyssey OLED G9 is just a hair over $1000 today, and it looks 
 like the price is right.The Latest Tech News, Delivered to Your Inbox.</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>6 hours ago</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>MSN</t>
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="inlineStr">
         <is>
           <t>https://it.chosun.com/news/articleView.html?idxno=2023092119303</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>Fascinating and Useful Hovering Hologram [Inho's Startup Pick]</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>To view something using electronic devices, an output device like a monitor 
 is needed. Even smartphones display content through an LCD screen.</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>6 days ago</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>IT조선</t>
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="30">
+      <c r="A30" t="inlineStr">
         <is>
           <t>https://tech.hindustantimes.com/gaming/news/gta-6-trailer-sparks-fan-analysis-san-andreas-vr-rumours-resurface-71720811864890.html</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>GTA 6 trailer sparks fan analysis; San Andreas VR rumours resurface-</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>Grand Theft Auto 6 first trailer has fans analysing every detail, while 
 recent comments from Video Games Deluxe reignite speculation about a VR 
 port for...</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>3 days ago</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>HT Tech</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+    <row r="31">
+      <c r="A31" t="inlineStr">
         <is>
           <t>https://www.newelectronics.co.uk/content/news/omnivision-unveils-shutter-image-sensor-for-arvrmr-tracking-cameras/</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>OMNIVISION unveils shutter image sensor for AR/VR/MR tracking cameras</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>OMNIVISION, a developer of advanced digital imaging, analogue, and touch &amp; 
 display technology, has launched the OG0TC BSI global shutter (GS) image 
 sensor.</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>1 week ago</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>New Electronics</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>https://www.msn.com/en-us/news/technology/meta-holographic-glasses-are-almost-ready-to-demo/ar-BB1p5o3o?item=themed_featuredapps_enabled?loadin</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Meta holographic glasses are almost ready to demo</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Meta's holographic AR glasses prototype is "almost ready" and could change 
-the tech landscape. The glasses will use transparent lenses to display...</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>4 days ago</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>MSN</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>https://www.msn.com/en-in/health/other/best-wearables-to-buy-for-yourself-top-10-picks-for-you-to-adopt-a-wire-free-lifestyle/ar-BB1pMw8p</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Best wearables to buy for yourself: Top 10 picks for you to adopt a 
-wire-free lifestyle</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Tired of tangled wires and cumbersome devices? Step into a world of 
-seamless connectivity and untethered freedom with the latest wearables.</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>3 days ago</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>MSN</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>https://www.openpr.com/news/3585153/volumetric-display-market-size-research-report-2024</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Volumetric Display Market Size Research Report 2024</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>USA, New Jersey: Volumetric Display Market was valued at USD 211.43 Million 
-in 2020 and is projected to reach USD 1549.19 Million by 2028,...</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>47 minutes ago</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>openPR.com</t>
         </is>
       </c>
     </row>
@@ -3131,7 +3105,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>21 hours ago</t>
+          <t>23 hours ago</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -3289,338 +3263,341 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>https://www.einnews.com/pr_news/728271630/holographic-ar-display-market-overview-2022-size-share-growth-trends-demand-forecast-report-2031</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Holographic AR Display Market Overview 2022 : Size, Share, Growth, Trends, 
+Demand, Forecast Report 2031</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Holographic AR Display Market," The holographic ar display market was 
+valued at $170.30 million in 2021, and is estimated to reach $2.6 billion 
+by 2031,...</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1 hour ago</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>EIN News</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>https://nocamels.com/2024/07/new-specs-augment-reality-and-make-you-look-good-doing-it/</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>New Specs Augment Reality And Make You Look Good Doing It</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Lumus Optics is using mirrors with a modern high-tech twist to help create 
 the cutting edge of stylish augmented reality (AR) glasses.</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>2 days ago</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>NoCamels</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="11">
+      <c r="A11" t="inlineStr">
         <is>
           <t>https://www.japantimes.co.jp/news/2024/07/16/world/society/ar15-america-popular-guns/</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>The AR-15: One of America's most popular and deadliest guns</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>The attempted assassination of former U.S. President Donald Trump with a 
 semiautomatic rifle illustrates once again how easy it is for shooters in 
 the U.S....</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>1 day ago</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>The Japan Times</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="inlineStr">
         <is>
           <t>https://www.macworld.com/article/557878/apple-vision-pro-features-specs-price-faq.html</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>Apple Vision Pro guide: Everything you need to know</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Having launched in the U.S. in February, Apple Vision Pro is now available 
 to buy in the U.K., Canada and elsewhere. Here's what you should know 
 about...</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>4 days ago</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>Macworld</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="13">
+      <c r="A13" t="inlineStr">
         <is>
           <t>https://magazine.cim.org/en/news/2024/underground-surveying-gets-an-ar-upgrade-en/</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>Underground surveying gets an AR upgrade</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>NSS Canada, a Sudbury, Ontario-based mining technology company, has 
 incorporated an augmented reality (AR) display into its underground 
 surveying software.</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>5 days ago</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>CIM Magazine</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>https://www.openpr.com/news/3574492/windshield-ar-heads-up-displays-hud-market-size-demands-growth</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>Windshield AR Heads Up Displays HUD Market Size, Demands, Growth</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>Press release - WiseGuy Reports - Windshield AR Heads Up Displays HUD 
 Market Size, Demands, Growth Dynamics, Top Players and Global Forecast 
 2032...</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>6 days ago</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>openPR.com</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>https://www.wicz.com/story/51022484/Laser-Display-Technology-Market-Is-Likely-to-Experience-a-Strong-Growth-During-2024-2032/</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Laser Display Technology Market Is Likely to Experience a Strong Growth 
 During 2024-2032</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Laser Display Technology Market Size 2024 To 2032 Laser Display Technology 
 Market Analysis [Latest 105 Report Pages with 20.12% CAGR]| by Product 
 Type...</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>6 days ago</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>WICZ</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="16">
+      <c r="A16" t="inlineStr">
         <is>
           <t>https://www.msn.com/en-us/news/us/new-greenway-section-opening-in-huntersville-with-unique-light-art-display/ar-BB1pSYck</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>New greenway section opening in Huntersville with unique light art display</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>The newest section of greenway in Mecklenburg County is opening next week, 
 and it's got a colorful surprise in it.</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>4 days ago</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>MSN</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>https://www.telecomlead.com/smart-phone/xr-industry-developments-and-near-eye-display-market-outlook-117090</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>XR industry developments and near-eye display market outlook</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>Kimi Lin and a team of analysts at Omdia have published a report on the 
 growth potential of the near-eye display market.</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>5 days ago</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>TelecomLead</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://www.msn.com/en-us/news/technology/i-have-no-problem-with-a-cheaper-vision-pro-having-a-worse-display/ar-BB1pfjDB?item=flightsprg-tipsubsc-v1a?loadin</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>I have no problem with a cheaper Vision Pro having a worse display</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Rumors point to Apple's cheaper Vision Pro headset coming with a worse 
+display, but that's fine by me.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2 days ago</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>MSN</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
         <is>
           <t>https://www.einnews.com/pr_news/726742643/display-market-is-expected-to-grow-from-157-8-billion-2023-to-reach-207-79-billion-in-2031-skyquest-technology</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>Display Market is Expected to Grow from 157.8 Billion 2023 to reach 207.79 
 Billion in 2031 | SkyQuest</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>WESTFORD, MASSACHUSETTS, UNITED STATES, July 11, 2024 /EINPresswire.com/ -- 
 Display Market size was valued at USD 152.46 billion in 2022 and is 
 expected to...</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>5 days ago</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>EIN News</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>https://www.msn.com/en-us/news/technology/i-have-no-problem-with-a-cheaper-vision-pro-having-a-worse-display/ar-BB1pfjDB?item=flightsprg-tipsubsc-v1a?loadin</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>I have no problem with a cheaper Vision Pro having a worse display</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Rumors point to Apple's cheaper Vision Pro headset coming with a worse 
-display, but that's fine by me.</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2 days ago</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>MSN</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+    <row r="20">
+      <c r="A20" t="inlineStr">
         <is>
           <t>https://www.msn.com/en-us/music/news/grammy-museum-to-display-bts-seventeen-and-more-hybe-artists-memorabilia/ar-BB1pHeBT</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>Grammy Museum to Display BTS, Seventeen and More HYBE Artists' Memorabilia</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>Hybe — the Korean firm behind BTS, Seventeen, Tomorrow x Together and more 
 — is getting a big look at the Grammy Museum in Downtown Los Angeles.</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>6 days ago</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>MSN</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>https://www.msn.com/en-us/news/technology/how-to-change-display-orientation-in-windows/ar-AA1eS0pE?item=flights%3Cimg%20src&amp;item=flights%3Cimg%20&amp;item=flights%3Cimg%20src&amp;item=flights%3Cimg%20</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>How to Change Display Orientation in Windows</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Need to flip or rotate your computer screen? Here's how to do so on Windows.</t>
-        </is>
-      </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12 hours ago</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -3632,311 +3609,310 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>https://www.msn.com/en-us/news/technology/how-to-change-display-orientation-in-windows/ar-AA1eS0pE?item=flights%3Cimg%20src&amp;item=flights%3Cimg%20&amp;item=flights%3Cimg%20src&amp;item=flights%3Cimg%20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>How to Change Display Orientation in Windows</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Need to flip or rotate your computer screen? Here's how to do so on Windows.</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>14 hours ago</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>MSN</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>https://www.msn.com/en-us/news/world/sycamore-gap-trunk-rings-art-goes-on-display/ar-BB1pZf8j?ocid=BingNewsVerp</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>Sycamore Gap trunk-rings art goes on display</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>A collection of five prints created from the trunk of the Sycamore Gap tree 
 have gone on public display. The 200-year-old tree, which towered 50ft 
 above...</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>1 day ago</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2 days ago</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>MSN</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
+    <row r="23">
+      <c r="A23" t="inlineStr">
         <is>
           <t>https://www.msn.com/en-us/lifestyle/shopping/jbl-s-new-earbuds-have-a-display-built-into-the-charging-case-but-that-s-not-their-best-feature/ar-BB1pBXPR</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>JBL's new earbuds have a display built into the charging case, but that's 
 not their best feature</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>retail for $200 and deliver fantastic audio playback, reliable noise 
 cancellation, and great battery life. The earbuds should satisfy most users 
 with their...</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>5 hours ago</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>7 hours ago</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>MSN</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="24">
+      <c r="A24" t="inlineStr">
         <is>
           <t>https://www.lelezard.com/en/news-21453722.html</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>AR/VR/MR Market Revolutionizing Industries: Pathway to Surpassing USD 
 521.28 Billion by 2031 | SkyQuest</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>According to SkyQuest, the global, AR/VR/MR Market size was valued at USD 
 30.6 Billion in 2022 and is poised to grow from USD 42.46 Billion in 2023 
 to USD...</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>18 hours ago</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>20 hours ago</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>Lelezard</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>https://www.msn.com/en-us/news/technology/microsoft-patents-a-technique-to-display-encrypted-documents-so-only-you-can-see-them/ar-BB1pteOP?item=flightsprg-tipsubsc-v1a?loadIn=defaultBrowser</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://www.msn.com/en-us/news/technology/microsoft-patents-a-technique-to-display-encrypted-documents-so-only-you-can-see-them/ar-BB1pteOP?item=flightsprg-tipsubsc-v1a?season89c26d1ce19649ab8c6b1ea6904de419thu</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>Microsoft patents a technique to display encrypted documents so only you 
 can see them</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>It seems to be a better system than AMD's Privacy View feature but like all 
 of them, it can't solve one key issue.</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>16 hours ago</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>8 hours ago</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>MSN</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://www.msn.com/en-us/lifestyle/shopping/google-pixel-watch-3-tipped-for-massive-display-upgrade-what-you-need-to-know/ar-BB1pLFSn?ocid=BingNewsVerp</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Google Pixel Watch 3 tipped for massive display upgrade — what you need to 
+know</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Google's Pixel Watch 3 is rumored to get several significant display 
+upgrades, making it a massive leap over the Pixel Watch 2.</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>6 days ago</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>MSN</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
         <is>
           <t>https://www.msn.com/en-us/news/us/star-wars-costumes-and-props-go-on-display-in-greenville/ar-BB1obuvi?ocid=BingNewsVerp</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>'Star Wars' costumes and props go on display in Greenville</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>Starting Saturday, June 15, fans can see a collection of costumes and props 
 from the "Star Wars" movies in Greenville.</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>6 days ago</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>MSN</t>
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>https://www.msn.com/en-us/lifestyle/shopping/google-pixel-watch-3-tipped-for-massive-display-upgrade-what-you-need-to-know/ar-BB1pLFSn?ocid=BingNewsVerp</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Google Pixel Watch 3 tipped for massive display upgrade — what you need to 
-know</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Google's Pixel Watch 3 is rumored to get several significant display 
-upgrades, making it a massive leap over the Pixel Watch 2.</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>6 days ago</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>MSN</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="28">
+      <c r="A28" t="inlineStr">
         <is>
           <t>https://www.msn.com/en-us/lifestyle/shopping/sony-launches-a-new-98-inch-bravia-display-with-non-glare-coating-and-hdr-support-price-features-and-more/ar-BB1pEy3W?ocid=BingNewsVerp</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>Sony launches a new 98-inch Bravia display with non-glare coating and HDR 
 support: Price, features and more</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>Sony India unveils the 98-inch BZ53L BRAVIA display featuring Deep Black 
 Non-Glare Coating, 4K HDR, 120 Hz, XR TRILUMINOS™ Pro, and Full Array Local 
 Dimming...</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>3 days ago</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>MSN</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="inlineStr">
         <is>
           <t>https://www.msn.com/en-us/travel/news/planes-and-stories-wwii-era-planes-on-display-at-lunken-airport-to-honor-americas-past/ar-BB1pr5no?ocid=BingNewsVerp</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>Planes and stories: WWII-era planes on display at Lunken Airport to honor 
 America's past</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>People are celebrating the ingenuity, courage, and determination of those 
 Americans who came before us this Independence Day weekend.</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>3 days ago</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>MSN</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
+    <row r="30">
+      <c r="A30" t="inlineStr">
         <is>
           <t>https://www.msn.com/en-us/news/technology/full-amd-ryzen-pc-crammed-into-a-folding-mini-keyboard-includes-a-built-in-trackpad-and-battery-all-you-need-is-a-display/ar-BB1pyUEm?item=flights%3Cimg%20src&amp;item=flights%3Cimg%20src&amp;item=flights%3Cimg%20src&amp;item=flights%3Cimg%20src</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>Full AMD Ryzen PC crammed into a folding mini keyboard — includes a 
 built-in trackpad and battery; all you need is a display</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>Chinese PC maker Linglong has just introduced a tiny PC that fits into a 
 foldable keyboard. The company shared its live presentation, where the 
 presenter...</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>5 days ago</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>MSN</t>
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
+    <row r="31">
+      <c r="A31" t="inlineStr">
         <is>
           <t>https://www.msn.com/en-us/lifestyle/lifestyle-buzz/meaning-behind-meghan-markle-s-constant-harry-hand-holding-amid-smitten-display-at-espys/ar-BB1pRqmH</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>Meaning behind Meghan Markle's constant Harry hand holding amid smitten 
 display at ESPYs</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>The real meaning of Meghan Markle's constant hand holding with Prince Harry 
 has been revealed after their very loved-up display at the ESPY awards,...</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>3 days ago</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>MSN</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>https://www.msn.com/en-us/lifestyle/shopping/get-this-27-gaming-monitor-for-only-159-77-ar/ar-BB1pTU5n?item=themed_featuredapps_enableD</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Get This 27" Gaming Monitor for Only $159.77 AR</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>The ASRock 27" QHD 180Hz Gaming Monitor is currently on sale for $159.77 
-after rebate, marking the lowest price in the.</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -4015,7 +3991,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>18 hours ago</t>
+          <t>20 hours ago</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -4043,7 +4019,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>10 hours ago</t>
+          <t>12 hours ago</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -4248,7 +4224,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3 days ago</t>
+          <t>4 days ago</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -4393,7 +4369,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>18 hours ago</t>
+          <t>20 hours ago</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -4599,7 +4575,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>5 days ago</t>
+          <t>6 days ago</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -4772,7 +4748,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>4 days ago</t>
+          <t>5 days ago</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -4829,7 +4805,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4 hours ago</t>
+          <t>6 hours ago</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">

</xml_diff>